<commit_message>
Race sessions of different lengths now possible. Note: Mid-race events removed as a result.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="113">
   <si>
     <t>Section Text English</t>
   </si>
@@ -217,7 +217,8 @@
     <t>TeamSelectionUI, EnableRacing</t>
   </si>
   <si>
-    <t>Happy with where you’ve placed everyone? Don’t worry if you don’t get the perfect crew set-up on the first attempt, there’s four sets of practice races before the race proper, and you’ll get feedback on your choices after each.
+    <t>Happy with where you’ve placed everyone? Don’t worry if you don’t get the perfect crew set-up on the first attempt, there’s usually four sets of practice races before the race proper, and you’ll get feedback on your choices after each.
+Keep in mind though, for this tutorial you'll only be given two practice sessions.
 A team's performance is based on the crew member’s ratings in the skills needed for the position, their opinion of you, their opinion of everyone else in a position and their current mood.
 Click the highlighted button and your current crew will take part in their first practice session.</t>
   </si>
@@ -278,22 +279,10 @@
     <t>Passando sopra le icone blue puoi vedere quali aree devi migliorare.</t>
   </si>
   <si>
-    <t>That's the first practice session completed. You now have three more sessions which to experiement in before the race itself.</t>
-  </si>
-  <si>
-    <t>La prima sessione di prova è conclusa. Hai ancora 3 sessioni di prova prima della gara vera e propria.</t>
-  </si>
-  <si>
-    <t>That's two more practice sessions down. Two more to go!</t>
-  </si>
-  <si>
-    <t>Due sessioni di prova sono concluse. Ancora due prove prima di partire!</t>
-  </si>
-  <si>
-    <t>Three sessions down. This'll be your last chance to experiment risk-free, so pick wisely.</t>
-  </si>
-  <si>
-    <t>Tre sessioni sono concluse. Questa è la tua ultima possibilità per provare senza rischio, quindi cerca di fare una scelta saggia.</t>
+    <t>That's the first practice session completed. This'll be your last chance to experiment risk-free, so pick wisely.</t>
+  </si>
+  <si>
+    <t>La prima sessione di prova è conclusa. Questa è la tua ultima possibilità per provare senza rischio, quindi cerca di fare una scelta saggia.</t>
   </si>
   <si>
     <t>OK, practice is over and it's now time for the race!
@@ -379,31 +368,22 @@
   </si>
   <si>
     <t>Now we’ve got someone that you feel fits this new position, it’s time to go into the next set of race session.
-As before, you’ve got four practice sessions and the race itself.
+As before, you’ve got only two practice sessions and the race itself.
 Feel free to ask all your team members further questions in interviews as well, if you wish.</t>
   </si>
   <si>
     <t>Ora hai qualcuno che ritieni possa ricoprire la nuova posizione, è tempo di passare alla sessione di gioco successiva.
-Come prima, hai 4 prove pratiche prima della gara vera e propria.
+Come prima, hai 2 prove pratiche prima della gara vera e propria.
 Puoi intervistare tutti I membri del tuo equipaggio se lo desideri.</t>
   </si>
   <si>
-    <t>That's the first practice session completed. You now have three more to experiement in before the race itself.</t>
-  </si>
-  <si>
-    <t>Hai appena completato la tua prima sessione di pratica. Hai ancora tre sessioni di prova prima di gareggiare.</t>
-  </si>
-  <si>
-    <t>Hai completato due sessioni di prova. Ne hai a disposizione ancora due!</t>
-  </si>
-  <si>
-    <t>Hai già effettuato tre sessioni di prova. Questa sarà la tua ultima possibilità di sperimentare senza rischi, in modo da poter poi scegliere con maggior consapevolezza.</t>
-  </si>
-  <si>
-    <t>Four practice sessions have come and gone, so now it's time to race for the first time with this new layout. Good luck!</t>
-  </si>
-  <si>
-    <t>Hai completato quattro sessioni di prova, è arrivato il momento di gareggiare per la prima volta con questa formazione. Buona fortuna!</t>
+    <t>Hai appena completato la tua prima sessione di pratica. Questa sarà la tua ultima possibilità di sperimentare senza rischi, in modo da poter poi scegliere con maggior consapevolezza.</t>
+  </si>
+  <si>
+    <t>Two practice sessions have come and gone, so now it's time to race for the first time with this new layout. Good luck!</t>
+  </si>
+  <si>
+    <t>Hai completato due sessioni di prova, è arrivato il momento di gareggiare per la prima volta con questa formazione. Buona fortuna!</t>
   </si>
   <si>
     <t>Did practice make perfect this time round?</t>
@@ -1157,7 +1137,7 @@
         <v>54</v>
       </c>
       <c r="D18" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E18" s="3" t="b">
         <v>1</v>
@@ -1271,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="3">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="I21" s="3" t="b">
         <v>1</v>
@@ -1363,7 +1343,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>1</v>
@@ -1381,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>29</v>
@@ -1405,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="G25" s="3" t="b">
         <v>0</v>
@@ -1426,22 +1406,22 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="D26" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E26" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="G26" s="3" t="b">
         <v>0</v>
@@ -1455,20 +1435,18 @@
       <c r="J26" s="3">
         <v>2.0</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="D27" s="1">
         <v>0.0</v>
@@ -1477,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="G27" s="3" t="b">
         <v>0</v>
@@ -1491,29 +1469,27 @@
       <c r="J27" s="3">
         <v>1.0</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="G28" s="3" t="b">
         <v>0</v>
@@ -1525,20 +1501,20 @@
         <v>1</v>
       </c>
       <c r="J28" s="3">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="D29" s="1">
         <v>0.0</v>
@@ -1547,29 +1523,31 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="G29" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I29" s="3" t="b">
         <v>1</v>
       </c>
       <c r="J29" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K29" s="3"/>
+        <v>-1.0</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="L29" s="3"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>86</v>
@@ -1581,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G30" s="3" t="b">
         <v>0</v>
@@ -1593,56 +1571,56 @@
         <v>1</v>
       </c>
       <c r="J30" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K30" s="3"/>
+        <v>1.0</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="L30" s="3"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D31" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E31" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="G31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I31" s="3" t="b">
         <v>1</v>
       </c>
       <c r="J31" s="3">
-        <v>-1.0</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>92</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D32" s="1">
         <v>0.0</v>
@@ -1651,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="G32" s="3" t="b">
         <v>0</v>
@@ -1666,22 +1644,22 @@
         <v>1.0</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="L32" s="3"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D33" s="1">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E33" s="3" t="b">
         <v>1</v>
@@ -1699,17 +1677,17 @@
         <v>1</v>
       </c>
       <c r="J33" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>50</v>
@@ -1721,7 +1699,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="G34" s="3" t="b">
         <v>0</v>
@@ -1735,29 +1713,27 @@
       <c r="J34" s="3">
         <v>1.0</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="D35" s="1">
         <v>0.0</v>
       </c>
       <c r="E35" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="G35" s="3" t="b">
         <v>0</v>
@@ -1769,31 +1745,29 @@
         <v>1</v>
       </c>
       <c r="J35" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="D36" s="1">
         <v>0.0</v>
       </c>
       <c r="E36" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="G36" s="3" t="b">
         <v>0</v>
@@ -1805,19 +1779,17 @@
         <v>1</v>
       </c>
       <c r="J36" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>50</v>
@@ -1826,10 +1798,10 @@
         <v>0.0</v>
       </c>
       <c r="E37" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="G37" s="3" t="b">
         <v>0</v>
@@ -1841,29 +1813,29 @@
         <v>1</v>
       </c>
       <c r="J37" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E38" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="G38" s="3" t="b">
         <v>0</v>
@@ -1881,140 +1853,33 @@
       <c r="L38" s="3"/>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E39" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G39" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I39" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="K39" s="3"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="F39" s="2"/>
       <c r="L39" s="3"/>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E40" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G40" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I40" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="F40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E41" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G41" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H41" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I41" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J41" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="F41" s="2"/>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E42" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G42" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I42" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J42" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43">
       <c r="A43" s="2"/>
@@ -2022,7 +1887,6 @@
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="L43" s="3"/>
     </row>
     <row r="44">
       <c r="A44" s="2"/>
@@ -8786,34 +8650,6 @@
       <c r="D1009" s="2"/>
       <c r="F1009" s="2"/>
     </row>
-    <row r="1010">
-      <c r="A1010" s="2"/>
-      <c r="B1010" s="2"/>
-      <c r="C1010" s="2"/>
-      <c r="D1010" s="2"/>
-      <c r="F1010" s="2"/>
-    </row>
-    <row r="1011">
-      <c r="A1011" s="2"/>
-      <c r="B1011" s="2"/>
-      <c r="C1011" s="2"/>
-      <c r="D1011" s="2"/>
-      <c r="F1011" s="2"/>
-    </row>
-    <row r="1012">
-      <c r="A1012" s="2"/>
-      <c r="B1012" s="2"/>
-      <c r="C1012" s="2"/>
-      <c r="D1012" s="2"/>
-      <c r="F1012" s="2"/>
-    </row>
-    <row r="1013">
-      <c r="A1013" s="2"/>
-      <c r="B1013" s="2"/>
-      <c r="C1013" s="2"/>
-      <c r="D1013" s="2"/>
-      <c r="F1013" s="2"/>
-    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Minor tutorial changes, system added for taking in custom tutorial attributes, talk time cost now not taken only when custom attribute is set.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
   <si>
     <t>Section Text English</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Button Blacklist</t>
+  </si>
+  <si>
+    <t>Custom Attributes</t>
   </si>
   <si>
     <t>Welcome to the Team Management screen!
@@ -77,6 +80,9 @@
   </si>
   <si>
     <t>PositionUI, ShowPopUp</t>
+  </si>
+  <si>
+    <t>cost=true</t>
   </si>
   <si>
     <t>This pop-up provides a list of skills required for the position you just selected, which should direct you toward who to pick for the next race once you know all the facts.
@@ -158,6 +164,9 @@
 Close (1)</t>
   </si>
   <si>
+    <t>cost=false</t>
+  </si>
+  <si>
     <t>OK, looks like you’ve got the hang of talking to a team member.
 Now you have some information for this crew member, exit this pop-up.</t>
   </si>
@@ -217,8 +226,8 @@
     <t>TeamSelectionUI, EnableRacing</t>
   </si>
   <si>
-    <t>Happy with where you’ve placed everyone? Don’t worry if you don’t get the perfect crew set-up on the first attempt, there’s usually four sets of practice races before the race proper, and you’ll get feedback on your choices after each.
-Keep in mind though, for this tutorial you'll only be given two practice sessions.
+    <t>Don’t worry if you haven't gotten the perfect line-up quite yet, as usually you'll get four sets of practice races before the race proper, with feedback on your choices after each.
+Keep in mind however that for this tutorial you'll only be given two practice sessions.
 A team's performance is based on the crew member’s ratings in the skills needed for the position, their opinion of you, their opinion of everyone else in a position and their current mood.
 Click the highlighted button and your current crew will take part in their first practice session.</t>
   </si>
@@ -258,9 +267,9 @@
     <t>HoverPopUpUI, HideHover</t>
   </si>
   <si>
-    <t>You'll also be given feedback on which areas your team is lacking in (if any).
-Ticks are a sign that you're on the right track toward selecting the most ideal line-up available to you.
-The grey question marks, meanwhile, display that information on how to improve your team is currently hidden to you.
+    <t>You'll also be given feedback on which areas your team needs to improve in (if any).
+Please note that, for this session only, these icons aren't representative of areas actually require improvement.
+The grey question marks, meanwhile, display information on how to improve your team is currently hidden to you.
 This information is revealed by further talking with your team about their skills and relationships with other crew members.
 By hovering over each of the blue icons, you can see what areas you need to improve in.</t>
   </si>
@@ -285,9 +294,9 @@
     <t>La prima sessione di prova è conclusa. Questa è la tua ultima possibilità per provare senza rischio, quindi cerca di fare una scelta saggia.</t>
   </si>
   <si>
-    <t>OK, practice is over and it's now time for the race!
+    <t>OK, practice is over and it's now time for the race itself!
 Do you play it safe and pick the best line-up from practice, or try and mix it up when it all matters?
-It’s up to you as their new manager…</t>
+Once you're happy with your selected line-up, click the 'Race!' button to take part in your first race.</t>
   </si>
   <si>
     <t xml:space="preserve">Ok, la pratica è finita; è arrivato il momento di gareggiare.
@@ -508,7 +517,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="76.86"/>
+    <col customWidth="1" min="1" max="1" width="45.57"/>
     <col customWidth="1" min="2" max="2" width="39.86"/>
     <col customWidth="1" min="3" max="3" width="30.86"/>
     <col customWidth="1" min="4" max="4" width="12.43"/>
@@ -553,7 +562,9 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -570,13 +581,13 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1">
         <v>3.0</v>
@@ -585,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="b">
         <v>0</v>
@@ -600,17 +611,19 @@
         <v>2.0</v>
       </c>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>0.0</v>
@@ -619,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3" t="b">
         <v>0</v>
@@ -634,17 +647,19 @@
         <v>1.0</v>
       </c>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1">
         <v>0.0</v>
@@ -653,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="b">
         <v>1</v>
@@ -668,17 +683,19 @@
         <v>2.0</v>
       </c>
       <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1">
         <v>0.0</v>
@@ -687,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3" t="b">
         <v>0</v>
@@ -702,17 +719,19 @@
         <v>1.0</v>
       </c>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1">
         <v>0.0</v>
@@ -721,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="3" t="b">
         <v>1</v>
@@ -736,17 +755,19 @@
         <v>2.0</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1">
         <v>0.0</v>
@@ -755,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G7" s="3" t="b">
         <v>0</v>
@@ -770,17 +791,19 @@
         <v>1.0</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1">
         <v>1.0</v>
@@ -789,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G8" s="3" t="b">
         <v>0</v>
@@ -804,19 +827,21 @@
         <v>0.0</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1">
         <v>0.0</v>
@@ -825,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" s="3" t="b">
         <v>0</v>
@@ -840,19 +865,21 @@
         <v>2.0</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1">
         <v>1.0</v>
@@ -861,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G10" s="3" t="b">
         <v>0</v>
@@ -876,17 +903,19 @@
         <v>1.0</v>
       </c>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1">
         <v>0.0</v>
@@ -895,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="b">
         <v>1</v>
@@ -910,19 +939,21 @@
         <v>0.0</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1">
         <v>0.0</v>
@@ -931,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G12" s="3" t="b">
         <v>0</v>
@@ -946,19 +977,21 @@
         <v>2.0</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1">
         <v>0.0</v>
@@ -967,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G13" s="3" t="b">
         <v>0</v>
@@ -982,17 +1015,19 @@
         <v>1.0</v>
       </c>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1">
         <v>0.0</v>
@@ -1001,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3" t="b">
         <v>1</v>
@@ -1016,19 +1051,21 @@
         <v>0.0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1">
         <v>0.0</v>
@@ -1037,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G15" s="3" t="b">
         <v>0</v>
@@ -1052,19 +1089,21 @@
         <v>2.0</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L15" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1">
         <v>0.0</v>
@@ -1073,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G16" s="3" t="b">
         <v>0</v>
@@ -1088,17 +1127,19 @@
         <v>1.0</v>
       </c>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1">
         <v>2.0</v>
@@ -1107,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G17" s="3" t="b">
         <v>0</v>
@@ -1122,19 +1163,21 @@
         <v>0.0</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1">
         <v>3.0</v>
@@ -1143,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G18" s="3" t="b">
         <v>0</v>
@@ -1158,17 +1201,19 @@
         <v>1.0</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1">
         <v>1.0</v>
@@ -1177,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G19" s="3" t="b">
         <v>1</v>
@@ -1192,17 +1237,19 @@
         <v>2.0</v>
       </c>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="L19" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D20" s="1">
         <v>0.0</v>
@@ -1211,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G20" s="3" t="b">
         <v>0</v>
@@ -1226,17 +1273,19 @@
         <v>1.0</v>
       </c>
       <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="L20" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1">
         <v>0.0</v>
@@ -1245,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G21" s="3" t="b">
         <v>1</v>
@@ -1260,17 +1309,19 @@
         <v>2.0</v>
       </c>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="L21" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1">
         <v>0.0</v>
@@ -1279,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G22" s="3" t="b">
         <v>0</v>
@@ -1294,17 +1345,19 @@
         <v>1.0</v>
       </c>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="L22" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1">
         <v>0.0</v>
@@ -1313,7 +1366,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G23" s="3" t="b">
         <v>0</v>
@@ -1328,19 +1381,21 @@
         <v>1.0</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L23" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D24" s="1">
         <v>2.0</v>
@@ -1349,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G24" s="3" t="b">
         <v>0</v>
@@ -1364,19 +1419,21 @@
         <v>2.0</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L24" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1">
         <v>0.0</v>
@@ -1385,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G25" s="3" t="b">
         <v>0</v>
@@ -1400,19 +1457,21 @@
         <v>1.0</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L25" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D26" s="1">
         <v>1.0</v>
@@ -1421,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G26" s="3" t="b">
         <v>0</v>
@@ -1436,17 +1495,19 @@
         <v>2.0</v>
       </c>
       <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="L26" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1">
         <v>0.0</v>
@@ -1455,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G27" s="3" t="b">
         <v>0</v>
@@ -1470,17 +1531,19 @@
         <v>1.0</v>
       </c>
       <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="L27" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D28" s="1">
         <v>0.0</v>
@@ -1489,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G28" s="3" t="b">
         <v>0</v>
@@ -1504,17 +1567,19 @@
         <v>0.0</v>
       </c>
       <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="L28" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D29" s="1">
         <v>0.0</v>
@@ -1523,7 +1588,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G29" s="3" t="b">
         <v>1</v>
@@ -1538,19 +1603,21 @@
         <v>-1.0</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L29" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="D30" s="1">
         <v>0.0</v>
@@ -1559,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G30" s="3" t="b">
         <v>0</v>
@@ -1574,19 +1641,21 @@
         <v>1.0</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L30" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D31" s="1">
         <v>2.0</v>
@@ -1595,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G31" s="3" t="b">
         <v>0</v>
@@ -1610,17 +1679,19 @@
         <v>1.0</v>
       </c>
       <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="L31" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D32" s="1">
         <v>0.0</v>
@@ -1629,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G32" s="3" t="b">
         <v>0</v>
@@ -1644,19 +1715,21 @@
         <v>1.0</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L32" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D33" s="1">
         <v>0.0</v>
@@ -1665,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G33" s="3" t="b">
         <v>0</v>
@@ -1680,17 +1753,19 @@
         <v>2.0</v>
       </c>
       <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+      <c r="L33" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D34" s="1">
         <v>0.0</v>
@@ -1699,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G34" s="3" t="b">
         <v>0</v>
@@ -1714,17 +1789,19 @@
         <v>1.0</v>
       </c>
       <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
+      <c r="L34" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D35" s="1">
         <v>0.0</v>
@@ -1733,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G35" s="3" t="b">
         <v>0</v>
@@ -1748,17 +1825,19 @@
         <v>3.0</v>
       </c>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="L35" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D36" s="1">
         <v>0.0</v>
@@ -1767,7 +1846,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G36" s="3" t="b">
         <v>0</v>
@@ -1782,17 +1861,19 @@
         <v>2.0</v>
       </c>
       <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
+      <c r="L36" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D37" s="1">
         <v>0.0</v>
@@ -1801,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G37" s="3" t="b">
         <v>0</v>
@@ -1816,17 +1897,19 @@
         <v>1.0</v>
       </c>
       <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
+      <c r="L37" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D38" s="1">
         <v>2.0</v>
@@ -1835,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G38" s="3" t="b">
         <v>0</v>
@@ -1850,7 +1933,9 @@
         <v>1.0</v>
       </c>
       <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
+      <c r="L38" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2"/>

</xml_diff>

<commit_message>
Tutorial updated to improve further description of some elements and reduce overall length greatly.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
   <si>
     <t>Section Text English</t>
   </si>
@@ -67,9 +67,8 @@
   <si>
     <t>Welcome to the Team Management screen!
 Here is where you’ll be dealing with your crew and assigning them their positions for races.
-Before we begin to get into the nitty-gritty of that though, let’s take a look at the three positions you’ll need to fill on your first boat.
-These three positions will need to be filled before you’ll be able to race on the open water.
-Click on any of them, and you’ll be given some tips on what kind of person will fit in better in that role.</t>
+Firstly, let’s take a look at the three positions you’ll need to fill.
+Click on any of them to display the pop-up for that position.</t>
   </si>
   <si>
     <t>Benvenuto nell'area di Gestione della squadra!
@@ -85,9 +84,8 @@
     <t>cost=true</t>
   </si>
   <si>
-    <t>This pop-up provides a list of skills required for the position you just selected, which should direct you toward who to pick for the next race once you know all the facts.
-This pop-up will eventually also display who’s currently in the position and has been in it in the past, but as the first race hasn’t happened, let’s not worry about that quite yet.
-Now close this pop-up using the X in the top right.</t>
+    <t>This pop-up lists all the skills required for the position you just selected and will, after your first race, also display who is currently in this position and has been in it the most in the past.
+To close this pop-up, use the X in the top right.</t>
   </si>
   <si>
     <t>Questa finestra ti mostra la lista delle competenze richieste per la posizione che hai appena selezionato. Tali competenze dovrebbero darti un'indicazione di chi selezionare per la prossima gara una volta raccolte tutte le informazioni.
@@ -101,27 +99,10 @@
     <t>PositionDisplayUI, ClosePositionPopUp</t>
   </si>
   <si>
-    <t>That's one of the positions reviewed. Click on either of the other two positions to continue looking into the skills required for your first crew.</t>
-  </si>
-  <si>
-    <t>Questa è una delle posizioni che è stata esaminata. Clicca su una delle due posizioni rimanenti per continuare a guardare le competenze richieste per il tuo primo equipaggio.</t>
-  </si>
-  <si>
-    <t>As before, once you're done close the pop-up using the X in the top right.</t>
-  </si>
-  <si>
-    <t>Come prima, una volta che hai finito chiudi la finestra usando la X in alto a destra.</t>
-  </si>
-  <si>
-    <t>That's two of the positions looked at now. Click on the final position to finish off the review of boat positions.</t>
-  </si>
-  <si>
-    <t>Queste sono due delle posizioni visionate. Clicca sull'ultima posizione per finire di esaminare le posizioni della barca.</t>
-  </si>
-  <si>
-    <t>Now that you know what positions need to be filled, it’s time to take a look at the crew you’re starting with.
-At the bottom of the screen, your six current crew members are listed.
-Simply click on any of them to go to the meeting screen for that crew member.</t>
+    <t>Now that you know how to review positions, it’s time to take a look at the crew you’re starting with. At the bottom of the screen, all your crew members are listed.
+The facial expression of each shows their current mood. At the moment all your crew is in a 'neutral' mood, which has no impact on their performance.
+A happy looking, smiling crew member will be in a good mood and as such will perform better than normal, whilst anyone looking sad or angry will be in a bad mood and will perform worse. 
+In order to find out more on a crew member, you'll need to talk to them, which you can do by clicking on them.</t>
   </si>
   <si>
     <t>Ora che conosci quali posizioni devono essere occupate, è tempo di dare un'occhiata all'equipaggio di partenza.
@@ -138,12 +119,10 @@
     <t>zz Recruit</t>
   </si>
   <si>
-    <t>This pop-up displays all the details you know for this crew member.
-As you’ve only just started and haven’t spoken to them yet, you know nothing about their skills and, as far as you’re aware, their opinion of everyone is neutral.
-In order to learn more about this crew member, you’re going to need to have a meeting with them.
-Simply click any of the available questions to ask them to this crew member.
-In the top left, responses from the crew member will be displayed after each question.
-Usually you’ll be capped on how many questions you can ask per race, but for now that limit has been removed, so feel free to ask each question a couple of times.</t>
+    <t>This pop-up displays all the known skills and opinions for this person, but as you’ve only just started, you know nothing about their skills and, as far as you’re aware, their opinion of everyone is neutral.
+Their opinion on other members of the team is displayed in the top left of their respective icons, whilst their opinion of you is shown in the top left of this pop-up. As known information on opinions becomes older, the backgrounds of these icons will also get progressively darker.
+In order to learn more about this crew member, you’re going to need to talk to them by clicking any of the available questions, with their response displayed above the list of questions.
+Asking questions, along with some other actions in the game, require an amount of 'Talk Time' to do, with a limited amount available per race. For now, this limitation has been removed, so feel free to ask each question a couple of times.</t>
   </si>
   <si>
     <t>Questa finestra mostra tutti I dettagli che conosci di questo membro dell'equipaggio.
@@ -167,8 +146,8 @@
     <t>cost=false</t>
   </si>
   <si>
-    <t>OK, looks like you’ve got the hang of talking to a team member.
-Now you have some information for this crew member, exit this pop-up.</t>
+    <t>OK, looks like you’ve got the hang of talking to your team.
+Now you have some information for this crew member, exit the pop-up using the highlighted button.</t>
   </si>
   <si>
     <t>Ok, sembra che tu abbia concluso di intervistare il membro dell'equipaggio.
@@ -181,39 +160,10 @@
     <t>MemberMeetingUI, OnDisable</t>
   </si>
   <si>
-    <t>In order to get to know your crew better, repeat this process for another crew member.
-As before, click on any of the crew members and you'll be able to question them.</t>
-  </si>
-  <si>
-    <t>Per conoscere meglio il tuo equipaggio intervista un altro membro.
-Come prima, clicca su una persona e sarai in grado di porgli delle domande.</t>
-  </si>
-  <si>
-    <t>As before, these questions will cost you no time, so free feel to ask away.</t>
-  </si>
-  <si>
-    <t>Come prima, queste domande non ti costeranno tempo, così sentiti libero di chiedere ciò che vuoi.</t>
-  </si>
-  <si>
-    <t>Now you've asked a few questions, leave this pop-up using the highlighted close button.</t>
-  </si>
-  <si>
-    <t>Ora hai fatto alcune domande, abbandona questa finestra usando il pulsante di chiusura evidenziato.</t>
-  </si>
-  <si>
-    <t>That's two crew members thoroughly questioned. You'll need to fill three positions, so pick a third crew member to find out further information for.</t>
-  </si>
-  <si>
-    <t>Ora hai approfondito la conoscenza con due membri dell'equipaggio. Dovrai ricoprire tre posizioni, quindi seleziona un terzo membro per scoprire ulteriori informazioni.</t>
-  </si>
-  <si>
-    <t>Come prima, le domande non ti costeranno del tempo, sentiti libero di andare avanti a chiedere.</t>
-  </si>
-  <si>
-    <t>Now you’ve questioned your crew, it’s time to place them in their positions.
-Using the information you’ve gathered from the position descriptions and crew member interviews, place crew members by dragging and dropping them into the position you think they’d best fit.
-If you want to remove a crew member from a position, just drag and drop them out of the position.
-Fill all of the positions wth crew members and the boat will be ready to take part in its first practice session.</t>
+    <t>Now you know how to question your crew, it’s time to place them into positions.
+Once you've gathered some further information on your team and the positions you'll need to find, place crew members by dragging them into the position you think they’d best fit.
+If you want to remove a crew member from a position, just drag them out of the position.
+Once you've filled all of the positions wth crew members, the boat will be ready to take part in the first practice session.</t>
   </si>
   <si>
     <t>Usando l'informazione che hai raccolto dalle interviste con I membri dell'equipaggio, disponi I candidati trascinandoli nelle posizioni che ritieni possano ricoprire meglio.
@@ -226,10 +176,10 @@
     <t>TeamSelectionUI, EnableRacing</t>
   </si>
   <si>
-    <t>Don’t worry if you haven't gotten the perfect line-up quite yet, as usually you'll get four sets of practice races before the race proper, with feedback on your choices after each.
+    <t>Don’t worry if you haven't gotten the perfect line-up, as usually you'll get four practice session before the race proper, with feedback on your choices after each session.
 Keep in mind however that for this tutorial you'll only be given two practice sessions.
-A team's performance is based on the crew member’s ratings in the skills needed for the position, their opinion of you, their opinion of everyone else in a position and their current mood.
-Click the highlighted button and your current crew will take part in their first practice session.</t>
+Every session, your performance is based on the skill ratings of your line-up in their positions, their opinion of you, their current mood and their opinion of everyone else selected.
+By clicking the highlighted button, yourr selected line-up will take part in the first practice session.</t>
   </si>
   <si>
     <t>Sei soddisfatto di come hai collocato ognuno? Non ti preoccupare se non individui la formazione perfetta al primo tentativo, ci sono 4 prove per fare pratica prima della gara vera propria. Riceverai un feedback sulle scelte fatte al termine di ciascuna prova.
@@ -243,9 +193,9 @@
     <t>TeamSelectionUI, ConfirmLineUp</t>
   </si>
   <si>
-    <t>After every race session, you'll be given feedback on how your selected crew performed.
-These colored boxes represent how many have been positioned compared to the ideal combination you could have created.
-Hover over each box to see what they represent.</t>
+    <t>After every session, you'll be given feedback on how your selected crew performed.
+These colored boxes represent how close you are to selecting the best possible line-up available to you.
+Hover over or click each box to see what they represent.</t>
   </si>
   <si>
     <t>I quadratini colorati rappresentano quanti membri sono stati posizionati rispetto alla disposizione ideale.
@@ -258,7 +208,7 @@
     <t>HoverPopUpUI, HoverCheck</t>
   </si>
   <si>
-    <t>Hover over each box to see what they represent.</t>
+    <t>Hover over or click each box to see what they represent.</t>
   </si>
   <si>
     <t>Posizionati su ciascun quadratino per leggere ciò che rappresenta.</t>
@@ -267,11 +217,11 @@
     <t>HoverPopUpUI, HideHover</t>
   </si>
   <si>
-    <t>You'll also be given feedback on which areas your team needs to improve in (if any).
-Please note that, for this session only, these icons aren't representative of areas actually require improvement.
-The grey question marks, meanwhile, display information on how to improve your team is currently hidden to you.
-This information is revealed by further talking with your team about their skills and relationships with other crew members.
-By hovering over each of the blue icons, you can see what areas you need to improve in.</t>
+    <t>You'll also be given feedback after every session on which areas your team needs to improve in, if any.
+Note that, for this session only, these icons aren't representative of which areas actually require improvement.
+Each blue icon represents an area that requires improvement, with icons on the left having more room for improvement.
+Grey question marks mean that your team needs to be questioned further in order to discover what needs improving.
+By hovering over each of the blue icons, you can see what each icon represents.</t>
   </si>
   <si>
     <t>Riceverai anche un feedback sulle aree in cui il tuo team è carente (se presenti).
@@ -282,20 +232,20 @@
     <t>Team Management/Boat Container Bounds/Viewport/Content/Historic Boat 0/Icon Container</t>
   </si>
   <si>
-    <t>By hovering over each of the blue icons, you can see what areas you need to improve in.</t>
+    <t>By hovering over each of the blue icons, you can see what each icon represents.</t>
   </si>
   <si>
     <t>Passando sopra le icone blue puoi vedere quali aree devi migliorare.</t>
   </si>
   <si>
-    <t>That's the first practice session completed. This'll be your last chance to experiment risk-free, so pick wisely.</t>
+    <t>Also keep in mind that selecting the best possible crew won't always mean you'll win the race. After all, the best of a poor crew is still going to be fairly bad.
+Now that you've completed the first practice session, use what you've learned to take part in the second practice session.</t>
   </si>
   <si>
     <t>La prima sessione di prova è conclusa. Questa è la tua ultima possibilità per provare senza rischio, quindi cerca di fare una scelta saggia.</t>
   </si>
   <si>
-    <t>OK, practice is over and it's now time for the race itself!
-Do you play it safe and pick the best line-up from practice, or try and mix it up when it all matters?
+    <t>OK, practice is over and it's now time for the race itself! Do you play it safe and pick based on what you know, or try and experiment when it matters?
 Once you're happy with your selected line-up, click the 'Race!' button to take part in your first race.</t>
   </si>
   <si>
@@ -304,7 +254,7 @@
 Spetta a te in quanto coach della squadra. </t>
   </si>
   <si>
-    <t>After every race, you'll be shown how your team performed in the last race. Did this one go as well as you expected in the end?</t>
+    <t>This result pop-up will apear after every race. Did this race go as well as you expected?</t>
   </si>
   <si>
     <t>Dopo ogni gara ti verrà mostrata la performance della tua  squadra  nell'ultima gara. Le cose sono andate come ti aspettavi?</t>
@@ -344,8 +294,7 @@
     <t>RecruitMemberUI, ResetDisplay</t>
   </si>
   <si>
-    <t>Here are your four options you have to recruit from.
-By clicking the skill statements at the bottom of the screen, all four will reply with if they agree or disagree with the statement offered.
+    <t>By clicking the skill statements at the bottom of the screen, these four possible recruits will reply with if they agree or disagree with the statement.
 By saying the right statements, you should get an idea on who to hire.
 Note that usually each of these questions would have a cost, as would hiring. This cost has been removed for the time being.</t>
   </si>
@@ -367,7 +316,7 @@
 Button</t>
   </si>
   <si>
-    <t>Once you’re happy that you know who you want to hire, simply click on them to hire them into your team.</t>
+    <t>Once you’re happy that you know who you want to hire, click on them to hire them into your team.</t>
   </si>
   <si>
     <t>Una volta che sei convinto su chi vuoi reclutare, è sufficiente cliccare sull'immagine per inserire il giocatore nella tua squadra.</t>
@@ -376,9 +325,8 @@
     <t>RecruitMemberUI, Recruit</t>
   </si>
   <si>
-    <t>Now we’ve got someone that you feel fits this new position, it’s time to go into the next set of race session.
-As before, you’ve got only two practice sessions and the race itself.
-Feel free to ask all your team members further questions in interviews as well, if you wish.</t>
+    <t>Now we’ve got someone that you feel fits the new position, it’s time for the next set of sessions.
+As before, you’ve got two practice sessions before the race itself.</t>
   </si>
   <si>
     <t>Ora hai qualcuno che ritieni possa ricoprire la nuova posizione, è tempo di passare alla sessione di gioco successiva.
@@ -386,6 +334,9 @@
 Puoi intervistare tutti I membri del tuo equipaggio se lo desideri.</t>
   </si>
   <si>
+    <t>That's the first practice session completed. This'll be your last chance to experiment risk-free, so pick wisely.</t>
+  </si>
+  <si>
     <t>Hai appena completato la tua prima sessione di pratica. Questa sarà la tua ultima possibilità di sperimentare senza rischi, in modo da poter poi scegliere con maggior consapevolezza.</t>
   </si>
   <si>
@@ -401,7 +352,7 @@
     <t>Pensi che la pratica che hai fatto ti aiuti ad affrontare il prossimo round?</t>
   </si>
   <si>
-    <t>Seems that one of your team members is wondering why they weren’t picked for that last race.
+    <t>Seems that one of your crew members wants to speak with you.
 Every so often, events like this will occur after a race, and it’s up to you to handle the situation.
 Click any of the available options to select and say them back to this crew member.</t>
   </si>
@@ -417,7 +368,7 @@
     <t>PostRaceEventUI, SetBlockerOnClick</t>
   </si>
   <si>
-    <t>OK, that’s the conversation finished. To exit and find out what effect this has had, click the highlighted button.</t>
+    <t>OK, that’s the conversation finished. Click the highlighted button to exit the conversation.</t>
   </si>
   <si>
     <t>OK, questa conversazione è finita. Per uscire e scoprire l'effetto delle tue scelte, fai clic sul pulsante evidenziato.</t>
@@ -429,7 +380,8 @@
     <t>PostRaceEventUI, Hide</t>
   </si>
   <si>
-    <t>This dashing fellow (no relation, I assure you...) will pop up after every event to give you some feedback on how you handled the situation.</t>
+    <t>This dashing fellow (no relation, I assure you...) will pop up after every event to give you some feedback on how you handled the situation.
+To close this feedback, click anywhere on the screen.</t>
   </si>
   <si>
     <t>Dopo ogni episodio apparirà un feedback su come hai gestito la situazione.</t>
@@ -438,9 +390,7 @@
     <t>LearningPillUI, ClosePill</t>
   </si>
   <si>
-    <t>OK, that's the tutorial finished!
-From here on out, you're mostly on your own, but I'll pop up from time to time after events to give additional tips.
-Good luck!</t>
+    <t>From here on out, you're mostly on your own, but I'll pop up from time to time after events to give additional tips. Good luck!</t>
   </si>
   <si>
     <t>Questo tutorial è finito! Da qui in avanti non ci sarò più ad aiutarti,  ma farò un salto di tanto in tanto per darti delle indicazioni. In bocca al lupo!</t>
@@ -455,20 +405,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -482,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -494,6 +454,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,7 +622,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1">
         <v>0.0</v>
@@ -668,34 +631,36 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
         <v>1.0</v>
       </c>
       <c r="I4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="K4" s="3"/>
+        <v>3.0</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="L4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1">
         <v>0.0</v>
@@ -704,46 +669,48 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="I5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="J5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K5" s="3"/>
+        <v>2.0</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="L5" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
         <v>1.0</v>
@@ -752,31 +719,31 @@
         <v>0</v>
       </c>
       <c r="J6" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G7" s="3" t="b">
         <v>0</v>
@@ -785,34 +752,36 @@
         <v>1.0</v>
       </c>
       <c r="I7" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K7" s="3"/>
+        <v>0.0</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="L7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G8" s="3" t="b">
         <v>0</v>
@@ -824,71 +793,67 @@
         <v>1</v>
       </c>
       <c r="J8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E9" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G9" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="3">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="I9" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="3">
         <v>2.0</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
+      <c r="A10" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G10" s="3" t="b">
         <v>0</v>
@@ -897,110 +862,106 @@
         <v>1.0</v>
       </c>
       <c r="I10" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="3">
         <v>1.0</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="E11" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="G11" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="3">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I11" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>44</v>
+      <c r="A12" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1">
         <v>0.0</v>
       </c>
       <c r="E12" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H12" s="3">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="I12" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1">
         <v>0.0</v>
       </c>
       <c r="E13" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G13" s="3" t="b">
         <v>0</v>
@@ -1009,110 +970,112 @@
         <v>1.0</v>
       </c>
       <c r="I13" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="3">
         <v>1.0</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="L13" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E14" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="3" t="b">
         <v>0</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="3" t="b">
-        <v>1</v>
       </c>
       <c r="H14" s="3">
         <v>1.0</v>
       </c>
       <c r="I14" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="3">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1">
         <v>0.0</v>
       </c>
       <c r="E15" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="G15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H15" s="3">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="I15" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E16" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G16" s="3" t="b">
         <v>0</v>
@@ -1121,34 +1084,34 @@
         <v>1.0</v>
       </c>
       <c r="I16" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="G17" s="3" t="b">
         <v>0</v>
@@ -1160,33 +1123,31 @@
         <v>1</v>
       </c>
       <c r="J17" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D18" s="1">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G18" s="3" t="b">
         <v>0</v>
@@ -1198,7 +1159,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3" t="s">
@@ -1207,49 +1168,51 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D19" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="G19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="H19" s="3">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="J19" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="K19" s="3"/>
+        <v>-1.0</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="L19" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1">
         <v>0.0</v>
@@ -1258,7 +1221,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="G20" s="3" t="b">
         <v>0</v>
@@ -1272,41 +1235,43 @@
       <c r="J20" s="3">
         <v>1.0</v>
       </c>
-      <c r="K20" s="3"/>
+      <c r="K20" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="L20" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D21" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E21" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="G21" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="3">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I21" s="3" t="b">
         <v>1</v>
       </c>
       <c r="J21" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
@@ -1315,13 +1280,13 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D22" s="1">
         <v>0.0</v>
@@ -1330,7 +1295,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="G22" s="3" t="b">
         <v>0</v>
@@ -1344,20 +1309,22 @@
       <c r="J22" s="3">
         <v>1.0</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="L22" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1">
         <v>0.0</v>
@@ -1366,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G23" s="3" t="b">
         <v>0</v>
@@ -1378,33 +1345,31 @@
         <v>1</v>
       </c>
       <c r="J23" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>2.0</v>
+      </c>
+      <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G24" s="3" t="b">
         <v>0</v>
@@ -1416,33 +1381,31 @@
         <v>1</v>
       </c>
       <c r="J24" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="D25" s="1">
         <v>0.0</v>
       </c>
       <c r="E25" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="G25" s="3" t="b">
         <v>0</v>
@@ -1454,33 +1417,31 @@
         <v>1</v>
       </c>
       <c r="J25" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>3.0</v>
+      </c>
+      <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D26" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="G26" s="3" t="b">
         <v>0</v>
@@ -1501,22 +1462,22 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D27" s="1">
         <v>0.0</v>
       </c>
       <c r="E27" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="G27" s="3" t="b">
         <v>0</v>
@@ -1537,22 +1498,22 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="D28" s="1">
         <v>0.0</v>
       </c>
       <c r="E28" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="G28" s="3" t="b">
         <v>0</v>
@@ -1564,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
@@ -1572,370 +1533,75 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="I29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" s="3">
-        <v>-1.0</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="L29" s="3"/>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E30" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G30" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I30" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="F30" s="2"/>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E32" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I32" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E33" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I33" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E34" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I34" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J34" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="F34" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E35" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I35" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J35" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="F35" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G36" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J36" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="F36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G37" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H37" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I37" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J37" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="F37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E38" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G38" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H38" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I38" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="F38" s="2"/>
     </row>
     <row r="39">
       <c r="A39" s="2"/>
@@ -1943,7 +1609,6 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="L39" s="3"/>
     </row>
     <row r="40">
       <c r="A40" s="2"/>
@@ -8665,76 +8330,6 @@
       <c r="D999" s="2"/>
       <c r="F999" s="2"/>
     </row>
-    <row r="1000">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="F1000" s="2"/>
-    </row>
-    <row r="1001">
-      <c r="A1001" s="2"/>
-      <c r="B1001" s="2"/>
-      <c r="C1001" s="2"/>
-      <c r="D1001" s="2"/>
-      <c r="F1001" s="2"/>
-    </row>
-    <row r="1002">
-      <c r="A1002" s="2"/>
-      <c r="B1002" s="2"/>
-      <c r="C1002" s="2"/>
-      <c r="D1002" s="2"/>
-      <c r="F1002" s="2"/>
-    </row>
-    <row r="1003">
-      <c r="A1003" s="2"/>
-      <c r="B1003" s="2"/>
-      <c r="C1003" s="2"/>
-      <c r="D1003" s="2"/>
-      <c r="F1003" s="2"/>
-    </row>
-    <row r="1004">
-      <c r="A1004" s="2"/>
-      <c r="B1004" s="2"/>
-      <c r="C1004" s="2"/>
-      <c r="D1004" s="2"/>
-      <c r="F1004" s="2"/>
-    </row>
-    <row r="1005">
-      <c r="A1005" s="2"/>
-      <c r="B1005" s="2"/>
-      <c r="C1005" s="2"/>
-      <c r="D1005" s="2"/>
-      <c r="F1005" s="2"/>
-    </row>
-    <row r="1006">
-      <c r="A1006" s="2"/>
-      <c r="B1006" s="2"/>
-      <c r="C1006" s="2"/>
-      <c r="D1006" s="2"/>
-      <c r="F1006" s="2"/>
-    </row>
-    <row r="1007">
-      <c r="A1007" s="2"/>
-      <c r="B1007" s="2"/>
-      <c r="C1007" s="2"/>
-      <c r="D1007" s="2"/>
-      <c r="F1007" s="2"/>
-    </row>
-    <row r="1008">
-      <c r="A1008" s="2"/>
-      <c r="B1008" s="2"/>
-      <c r="C1008" s="2"/>
-      <c r="D1008" s="2"/>
-      <c r="F1008" s="2"/>
-    </row>
-    <row r="1009">
-      <c r="A1009" s="2"/>
-      <c r="B1009" s="2"/>
-      <c r="C1009" s="2"/>
-      <c r="D1009" s="2"/>
-      <c r="F1009" s="2"/>
-    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Fixes for full screen blocker not working in tutorials, incorrect localized names being selected for mew games
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
@@ -170,7 +170,7 @@
 Se vuoi rimuovere un membro da una posizione, semplicemente trascinalo via da quella posizione.</t>
   </si>
   <si>
-    <t>null</t>
+    <t>Team Management</t>
   </si>
   <si>
     <t>TeamSelectionUI, EnableRacing</t>
@@ -179,7 +179,7 @@
     <t>Don’t worry if you haven't gotten the perfect line-up, as usually you'll get four practice session before the race proper, with feedback on your choices after each session.
 Keep in mind however that for this tutorial you'll only be given two practice sessions.
 Every session, your performance is based on the skill ratings of your line-up in their positions, their opinion of you, their current mood and their opinion of everyone else selected.
-By clicking the highlighted button, yourr selected line-up will take part in the first practice session.</t>
+By clicking the highlighted button, your selected line-up will take part in the first practice session.</t>
   </si>
   <si>
     <t>Sei soddisfatto di come hai collocato ognuno? Non ti preoccupare se non individui la formazione perfetta al primo tentativo, ci sono 4 prove per fare pratica prima della gara vera propria. Riceverai un feedback sulle scelte fatte al termine di ciascuna prova.
@@ -442,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -456,6 +456,9 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -466,7 +469,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -733,7 +736,7 @@
       <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="1">
@@ -837,7 +840,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -909,7 +912,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -951,7 +954,7 @@
       <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="1">
@@ -989,7 +992,7 @@
       <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="1">
@@ -1027,7 +1030,7 @@
       <c r="B15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="1">
@@ -1249,7 +1252,7 @@
       <c r="B21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="1">
@@ -1285,7 +1288,7 @@
       <c r="B22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="1">
@@ -1323,7 +1326,7 @@
       <c r="B23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="1">
@@ -1359,7 +1362,7 @@
       <c r="B24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="1">
@@ -1467,7 +1470,7 @@
       <c r="B27" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="1">
@@ -1503,7 +1506,7 @@
       <c r="B28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="1">

</xml_diff>

<commit_message>
Updated Italian translation. Minor changes made to UI based on feedback.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
@@ -10,22 +10,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="B2">
-      <text>
-        <t xml:space="preserve">Doesn't tell player to click on a position
-	-Ellis Spice</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
   <si>
@@ -71,8 +55,10 @@
 Click on any of them to display the pop-up for that position.</t>
   </si>
   <si>
-    <t>Benvenuto nell'area di Gestione della squadra!
-Qui è dove tu ti occupi del tuo equipaggio e assegni le persone alle loro posizioni per le gare.</t>
+    <t xml:space="preserve">Benvenuto nell'area di Gestione della squadra!
+Qui è dove tu ti occupi del tuo equipaggio e assegni le persone alle loro posizioni per le gare. 
+Prima di tutto dai un'occhiata ai tre ruoli che devi ricoprire. 
+Clicca su ciascuno per leggere una descrizione. </t>
   </si>
   <si>
     <t>Team Management/Boat Container Bounds/Viewport/Content/Boat/Position Container</t>
@@ -88,9 +74,8 @@
 To close this pop-up, use the X in the top right.</t>
   </si>
   <si>
-    <t>Questa finestra ti mostra la lista delle competenze richieste per la posizione che hai appena selezionato. Tali competenze dovrebbero darti un'indicazione di chi selezionare per la prossima gara una volta raccolte tutte le informazioni.
-Qui potresti anche trovare chi si trova attualmente nella posizione ed è stato in questa posizione in passato. In ogni caso finché la prima gara non è stata disputata non preoccuparti di questo.
-Ora chiudi la finestra usando la X in alto a destra.</t>
+    <t xml:space="preserve">Questa finestra ti mostra la lista delle competenze richieste per la posizione che hai appena selezionato. Dopo la prima gara, troverai anche chi occupa al momento quella posizione e chi l'ha ricoperta in passato. 
+Per chiudere la finestra, usa la x in alto a destra. </t>
   </si>
   <si>
     <t>Team Management/Pop-up Bounds/Position Pop-Up</t>
@@ -105,9 +90,10 @@
 In order to find out more on a crew member, you'll need to talk to them, which you can do by clicking on them.</t>
   </si>
   <si>
-    <t>Ora che conosci quali posizioni devono essere occupate, è tempo di dare un'occhiata all'equipaggio di partenza.
-Nella parte bassa dello schermo sono elencati I tuoi 6 membri correnti.
-Clicca su uno qualsiasi di loro per avviare una conversazione con lui/lei.</t>
+    <t xml:space="preserve">Ora che conosci quali posizioni devono essere occupate, è tempo di dare un'occhiata all'equipaggio di partenza. Nella parte bassa dello schermo sono elencati tutti i componenti della tua squadra. 
+L'espressione facciale di ciascuno mostra il suo stato d'animo corrente. In questo momento il tuo equipaggio si trova in uno stato d'animo neutrale, che non ha impatto sulla performance. 
+Un membro che appare felice e sorridente si troverà in un stato d'animo positivo e avrà una prestazione superiore alla norma, mentre uno che appare triste o arrabbiato avrà una prestazione peggiore.
+Clicca sul personaggio per conoscere di più su di lui/lei e avviare una conversazione. </t>
   </si>
   <si>
     <t>Team Management/Crew Container</t>
@@ -125,12 +111,10 @@
 Asking questions, along with some other actions in the game, require an amount of 'Talk Time' to do, with a limited amount available per race. For now, this limitation has been removed, so feel free to ask each question a couple of times.</t>
   </si>
   <si>
-    <t>Questa finestra mostra tutti I dettagli che conosci di questo membro dell'equipaggio.
-Poichè hai appena iniziato a giocare e non hai ancora parlato con nessuno, non sai nulla sulle competenze e da quanto ne sai le opinioni di tutti sono neutrali.
-Per imparare di più su questo membro dell'equipaggio, devi parlare con lui.
-Clicca su una delle domande disponibili per porgliela.
-In alto a sinistra verranno mostrate le sue risposte  alla tua domanda.
-Solitamente avrai un limite nel numero di domande che potrai porre per ciascuna gara, ma per il momento il limite è stato rimosso pertanto sentiti libero di fare ciascuna domanda anche un paio di volte.</t>
+    <t>Questa finestra mostra tutte le abilità e le opinioni conosciute di questa persona ma poiché hai appena iniziato, non sai ancora nulla sulle competenze che possiedono i membri della squadra e da quanto ne sai la loro opinione è neutrale.
+L'opinione nei confronti degli altri membri della squadra è mostrata in alto a sinistra delle rispettive icone, mentre la loro opinione nei tuoi confronti è riportata in alto a sinistra di questa finestra. Quando l'informazione sulle opinioni diventa obsoleta, lo sfondo di queste icone diventerà progressivamente più scuro. 
+Per imparare di più su un membro dell'equipaggio, devi parlare con lui, cliccando su una delle domande disponibili. La risposta verrà riportata sopra la lista delle domande. 
+Fare domande, così come altre azioni nel gioco, richiede una certa quantità di "Tempo di conversazione" che ha una quantità limitata per ciascuna gara. Per il momento il limite è stato rimosso pertanto sentiti libero di fare ciascuna domanda anche un paio di volte.</t>
   </si>
   <si>
     <t>Team Management/Pop-up Bounds/Meeting Pop-Up</t>
@@ -150,8 +134,8 @@
 Now you have some information for this crew member, exit the pop-up using the highlighted button.</t>
   </si>
   <si>
-    <t>Ok, sembra che tu abbia concluso di intervistare il membro dell'equipaggio.
-Ora hai qualche informazione su di lui, esci da questa finestra.</t>
+    <t xml:space="preserve">Ok, sembra che tu abbia concluso di intervistare il tuo equipaggio.
+Ora hai qualche informazione su questo membro della squadra, esci da questa finestra usando il pulsante evidenziato. </t>
   </si>
   <si>
     <t>Team Management/Pop-up Bounds/Meeting Pop-Up/Close</t>
@@ -166,8 +150,10 @@
 Once you've filled all of the positions wth crew members, the boat will be ready to take part in the first practice session.</t>
   </si>
   <si>
-    <t>Usando l'informazione che hai raccolto dalle interviste con I membri dell'equipaggio, disponi I candidati trascinandoli nelle posizioni che ritieni possano ricoprire meglio.
-Se vuoi rimuovere un membro da una posizione, semplicemente trascinalo via da quella posizione.</t>
+    <t xml:space="preserve">Ora conosci come intervistare i membri del equipaggio, è giunto il momento di assegnarli alle posizioni. 
+Dopo aver raccolto ancora qualche informazione sul tuo team e sulle posizioni da ricoprire, disponi i candidati trascinandoli nelle posizioni che ritieni possano ricoprire meglio.
+Se vuoi rimuovere un membro da una posizione, semplicemente trascinalo via da quella posizione.
+Quando hai coperto tutte le posizioni, la barca è pronta per affrontare la prima sessione di pratica. </t>
   </si>
   <si>
     <t>Team Management</t>
@@ -182,8 +168,9 @@
 By clicking the highlighted button, your selected line-up will take part in the first practice session.</t>
   </si>
   <si>
-    <t>Sei soddisfatto di come hai collocato ognuno? Non ti preoccupare se non individui la formazione perfetta al primo tentativo, ci sono 4 prove per fare pratica prima della gara vera propria. Riceverai un feedback sulle scelte fatte al termine di ciascuna prova.
-La performance del team si basa sui punteggi del membri nelle capacità richieste per ciascuna posizione, sull'opinione che hanno di te, sulla loro opinione rispetto alle posizioni altrui e sul loro stato d'animo corrente.
+    <t>Non ti preoccupare se non individui la formazione perfetta al primo tentativo, ci sono 4 prove per fare pratica prima della gara vera propria. Riceverai un feedback sulle scelte fatte al termine di ciascuna prova.
+Per questo tutorial avrai solo due prove pratiche. 
+In ogni sessione, la tua performance si basa sui punteggi dei membri rispetto alle capacità richieste per ciascuna posizione, sull'opinione che hanno di te, sul loro stato d'animo e sulla loro opinione rispetto agli altri membri selezionati. 
 Clicca il pulsante evidenziato e la tua squadra parteciperà alla prima sessione di prova.</t>
   </si>
   <si>
@@ -198,8 +185,9 @@
 Hover over or click each box to see what they represent.</t>
   </si>
   <si>
-    <t>I quadratini colorati rappresentano quanti membri sono stati posizionati rispetto alla disposizione ideale.
-Passa su ciascuno per leggere ciò che rappresenta.</t>
+    <t>Dopo ogni sessione riceverai un feedback sulla performance dell'equipaggio che hai selezionato. 
+I cerchietti colorati segnalano quanto ti sei avvicinato alla selezione della formazione ideale.
+Clicca o passa sopra ciascuno per leggere ciò che rappresenta.</t>
   </si>
   <si>
     <t>Team Management/Boat Container Bounds/Viewport/Content/Historic Boat 0/Light Container</t>
@@ -211,7 +199,7 @@
     <t>Hover over or click each box to see what they represent.</t>
   </si>
   <si>
-    <t>Posizionati su ciascun quadratino per leggere ciò che rappresenta.</t>
+    <t>Clicca o passa sopra ciascuno per leggere ciò che rappresenta.</t>
   </si>
   <si>
     <t>HoverPopUpUI, HideHover</t>
@@ -224,9 +212,11 @@
 By hovering over each of the blue icons, you can see what each icon represents.</t>
   </si>
   <si>
-    <t>Riceverai anche un feedback sulle aree in cui il tuo team è carente (se presenti).
-I segni di spunta ti indicano che sei sulla strada giusta nel selezionare il team ideale.
-Il punto di domanda in grigio indica che l'informazione su come migliorare il tuo team è al momento nascosta.</t>
+    <t xml:space="preserve">Al termine di ciascuna sessione, riceverai anche un feedback sulle aree in cui il tuo team è carente (se presenti).
+Nota che unicamente per questa sessione, queste icone non sono rappresentative delle aree che effettivamente richiedono un miglioramento. 
+Ciascuna icona azzurra rappresenta una dimensione che richiede un miglioramento. Le icone sulla sinistra hanno un margine di miglioramento maggiore. 
+I punti di domanda in grigio indicano che il tuo equipaggio deve essere intervistato ulteriormente per scoprire cosa è necessario migliorare. 
+Passando su ciascuna icona azzurra puoi leggere ciò che rappresenta. </t>
   </si>
   <si>
     <t>Team Management/Boat Container Bounds/Viewport/Content/Historic Boat 0/Icon Container</t>
@@ -235,29 +225,30 @@
     <t>By hovering over each of the blue icons, you can see what each icon represents.</t>
   </si>
   <si>
-    <t>Passando sopra le icone blue puoi vedere quali aree devi migliorare.</t>
+    <t>Passando sopra le icone azzurre puoi vedere quali aree devi migliorare.</t>
   </si>
   <si>
     <t>Also keep in mind that selecting the best possible crew won't always mean you'll win the race. After all, the best of a poor crew is still going to be fairly bad.
 Now that you've completed the first practice session, use what you've learned to take part in the second practice session.</t>
   </si>
   <si>
-    <t>La prima sessione di prova è conclusa. Questa è la tua ultima possibilità per provare senza rischio, quindi cerca di fare una scelta saggia.</t>
+    <t xml:space="preserve">Ricordati che selezionare la squadra migliore non significa sempre vincere la gara.
+Ora che hai completato la prima sessione di prova, usa ciò che hai imparato per prender parte alla seconda. </t>
   </si>
   <si>
     <t>OK, practice is over and it's now time for the race itself! Do you play it safe and pick based on what you know, or try and experiment when it matters?
 Once you're happy with your selected line-up, click the 'Race!' button to take part in your first race.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ok, la pratica è finita; è arrivato il momento di gareggiare.
-Gioca senza rischiare e seleziona la migliore delle formazioni che hai provato, oppure ricombina le risorse quando è la sola cosa che conta.
-Spetta a te in quanto coach della squadra. </t>
+    <t xml:space="preserve">Ok, la pratica è finita; è arrivato il momento di gareggiare!
+Giocherai senza rischiare selezionando in base a ciò che conosci o proverai a sperimentare quando vale la pena farlo?
+Quando sei soddisfatto della formazione che hai scelto, clicca sul pulsante "Gara!" per prender parte alla prima gara. </t>
   </si>
   <si>
     <t>This result pop-up will apear after every race. Did this race go as well as you expected?</t>
   </si>
   <si>
-    <t>Dopo ogni gara ti verrà mostrata la performance della tua  squadra  nell'ultima gara. Le cose sono andate come ti aspettavi?</t>
+    <t xml:space="preserve">Questa finestra con i risultati apparirà al termine di ciascuna gara. La gara è andata come ti aspettavi? </t>
   </si>
   <si>
     <t>TeamSelectionUI, ClosePostRacePopUp</t>
@@ -268,9 +259,9 @@
 As a result, you’ll need to recruit a new member into your team. But first, let’s look at the details behind this new position to fill.</t>
   </si>
   <si>
-    <t>Ora che hai completato la tua prima gara e visto come funziona, cambiamo un po' le cose.
+    <t xml:space="preserve">Ora che hai completato la tua prima gara e visto come funziona, cambiamo un po' le cose.
 Un navigatore non è più necessario sulla tua barca. Ora è necessario un timoniere, e nessuno del tuo equipaggio attuale ricopre questa posizione molto bene.
-Di conseguenza, sarà necessario reclutare un nuovo membro per la squadra. Ma prima, diamo un'occhiata ai dettagli di questa posizione per ricoprirla al meglio.</t>
+Di conseguenza, sarà necessario reclutare un nuovo membro per la squadra. Ma prima, diamo un'occhiata ai dettagli di questa posizione da ricoprire. </t>
   </si>
   <si>
     <t>Team Management/Boat Container Bounds/Viewport/Content/Boat/Position Container/Position 1</t>
@@ -299,10 +290,9 @@
 Note that usually each of these questions would have a cost, as would hiring. This cost has been removed for the time being.</t>
   </si>
   <si>
-    <t>Ecco le quattro opzioni su cui puoi operare il reclutamento. 
-Cliccando sulle affermazioni relative ad abilità possedute nella parte inferiore dello schermo, tutte e quattro le persone risponderanno se sono d'accordo o in disaccordo con l'affermazione selezionata.
-Selezionando le affermazioni corrette, dovresti farti un'idea su chi includere nella squadra.
-Ciascuna di queste domande avrebbe un costo. Tale costo è stato rimosso per il momento.</t>
+    <t xml:space="preserve">Cliccando le affermazioni relative alle competenze, nella parte bassa dello schermo, i candidati diranno quanto sono d'accordo o in disaccordo con l'affermazione. 
+Scegliendo l'affermazione giusta, dovresti farti un'idea di chi reclutare. 
+Nota che solitamente ciascuna di queste domande ha un costo, così come il reclutamento. Questo costo è stato rimosso per il momento. </t>
   </si>
   <si>
     <t>Team Management/Pop-up Bounds/Recruit Pop-Up</t>
@@ -319,7 +309,7 @@
     <t>Once you’re happy that you know who you want to hire, click on them to hire them into your team.</t>
   </si>
   <si>
-    <t>Una volta che sei convinto su chi vuoi reclutare, è sufficiente cliccare sull'immagine per inserire il giocatore nella tua squadra.</t>
+    <t>Una volta che sei convinto chi vuoi reclutare, è sufficiente cliccare sull'immagine per inserire il giocatore nella tua squadra.</t>
   </si>
   <si>
     <t>RecruitMemberUI, Recruit</t>
@@ -329,9 +319,8 @@
 As before, you’ve got two practice sessions before the race itself.</t>
   </si>
   <si>
-    <t>Ora hai qualcuno che ritieni possa ricoprire la nuova posizione, è tempo di passare alla sessione di gioco successiva.
-Come prima, hai 2 prove pratiche prima della gara vera e propria.
-Puoi intervistare tutti I membri del tuo equipaggio se lo desideri.</t>
+    <t>Ora hai qualcuno che ritieni possa ricoprire la nuova posizione, è tempo di passare al prossimo insieme di sessioni. 
+Come prima, hai 2 prove pratiche prima della gara vera e propria.</t>
   </si>
   <si>
     <t>That's the first practice session completed. This'll be your last chance to experiment risk-free, so pick wisely.</t>
@@ -343,7 +332,7 @@
     <t>Two practice sessions have come and gone, so now it's time to race for the first time with this new layout. Good luck!</t>
   </si>
   <si>
-    <t>Hai completato due sessioni di prova, è arrivato il momento di gareggiare per la prima volta con questa formazione. Buona fortuna!</t>
+    <t>Hai completato due sessioni di prova; è arrivato il momento di gareggiare per la prima volta con questa formazione. Buona fortuna!</t>
   </si>
   <si>
     <t>Did practice make perfect this time round?</t>
@@ -357,7 +346,7 @@
 Click any of the available options to select and say them back to this crew member.</t>
   </si>
   <si>
-    <t>Sembra che uno dei membri del team si stia chiedendo  perché non è stato scelto per l'ultima gara.
+    <t>Sembra che uno dei membri della squadra voglia parlare con te. 
 Ogni tanto, eventi simili a questo, si verificheranno dopo una gara, e tu sarai chiamato a gestire la situazione.
 Fai clic su una delle opzioni disponibili per selezionare ciò che vuoi dire a questa persona.</t>
   </si>
@@ -371,7 +360,7 @@
     <t>OK, that’s the conversation finished. Click the highlighted button to exit the conversation.</t>
   </si>
   <si>
-    <t>OK, questa conversazione è finita. Per uscire e scoprire l'effetto delle tue scelte, fai clic sul pulsante evidenziato.</t>
+    <t>OK, questa conversazione è finita. Per uscire dalla conversazione fai clic sul pulsante evidenziato.</t>
   </si>
   <si>
     <t>Team Management/Pop-up Bounds/Event Pop-Up/Solo/Close</t>
@@ -384,7 +373,8 @@
 To close this feedback, click anywhere on the screen.</t>
   </si>
   <si>
-    <t>Dopo ogni episodio apparirà un feedback su come hai gestito la situazione.</t>
+    <t xml:space="preserve">Questa persona comparirà al termine di ciascun evento per darti un feedback su come hai gestito la situazione. 
+Per chiudere questo feedback, clicca in qualunque punto dello schermo. </t>
   </si>
   <si>
     <t>LearningPillUI, ClosePill</t>
@@ -393,7 +383,7 @@
     <t>From here on out, you're mostly on your own, but I'll pop up from time to time after events to give additional tips. Good luck!</t>
   </si>
   <si>
-    <t>Questo tutorial è finito! Da qui in avanti non ci sarò più ad aiutarti,  ma farò un salto di tanto in tanto per darti delle indicazioni. In bocca al lupo!</t>
+    <t xml:space="preserve">Da qui in avanti giocherai per conto tuo, ma comparirò di tanto in tanto dopo gli eventi per darti ulteriori suggerimenti. In bocca al lupo! </t>
   </si>
   <si>
     <t>PositionUI, ShowPopUp
@@ -405,13 +395,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <name val="Arial"/>
+    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -442,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -452,14 +445,20 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,7 +548,7 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -558,26 +557,26 @@
       <c r="D2" s="1">
         <v>3.0</v>
       </c>
-      <c r="E2" s="3" t="b">
+      <c r="E2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="b">
+      <c r="G2" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>1.0</v>
       </c>
-      <c r="I2" s="3" t="b">
+      <c r="I2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="4">
         <v>2.0</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -585,7 +584,7 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -594,26 +593,26 @@
       <c r="D3" s="1">
         <v>0.0</v>
       </c>
-      <c r="E3" s="3" t="b">
+      <c r="E3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="b">
+      <c r="G3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>1.0</v>
       </c>
-      <c r="I3" s="3" t="b">
+      <c r="I3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="4">
         <v>1.0</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -621,7 +620,7 @@
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -630,28 +629,28 @@
       <c r="D4" s="1">
         <v>0.0</v>
       </c>
-      <c r="E4" s="3" t="b">
+      <c r="E4" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="3" t="b">
+      <c r="G4" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>1.0</v>
       </c>
-      <c r="I4" s="3" t="b">
+      <c r="I4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="4">
         <v>3.0</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -659,7 +658,7 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -668,28 +667,28 @@
       <c r="D5" s="1">
         <v>0.0</v>
       </c>
-      <c r="E5" s="3" t="b">
+      <c r="E5" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="3" t="b">
+      <c r="G5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
         <v>6.0</v>
       </c>
-      <c r="I5" s="3" t="b">
+      <c r="I5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="4">
         <v>2.0</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -697,7 +696,7 @@
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -706,26 +705,26 @@
       <c r="D6" s="1">
         <v>1.0</v>
       </c>
-      <c r="E6" s="3" t="b">
+      <c r="E6" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="3" t="b">
+      <c r="G6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>1.0</v>
       </c>
-      <c r="I6" s="3" t="b">
+      <c r="I6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="4">
         <v>1.0</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -733,37 +732,37 @@
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="1">
         <v>1.0</v>
       </c>
-      <c r="E7" s="3" t="b">
+      <c r="E7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="3" t="b">
+      <c r="G7" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <v>1.0</v>
       </c>
-      <c r="I7" s="3" t="b">
+      <c r="I7" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="4">
         <v>0.0</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -771,7 +770,7 @@
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -780,26 +779,26 @@
       <c r="D8" s="1">
         <v>3.0</v>
       </c>
-      <c r="E8" s="3" t="b">
+      <c r="E8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="3" t="b">
+      <c r="G8" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>1.0</v>
       </c>
-      <c r="I8" s="3" t="b">
+      <c r="I8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="4">
         <v>1.0</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -807,7 +806,7 @@
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -816,34 +815,34 @@
       <c r="D9" s="1">
         <v>1.0</v>
       </c>
-      <c r="E9" s="3" t="b">
+      <c r="E9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="3" t="b">
+      <c r="G9" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>3.0</v>
       </c>
-      <c r="I9" s="3" t="b">
+      <c r="I9" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="4">
         <v>2.0</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -852,26 +851,26 @@
       <c r="D10" s="1">
         <v>0.0</v>
       </c>
-      <c r="E10" s="3" t="b">
+      <c r="E10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="3" t="b">
+      <c r="G10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>1.0</v>
       </c>
-      <c r="I10" s="3" t="b">
+      <c r="I10" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="4">
         <v>1.0</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -879,7 +878,7 @@
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -888,34 +887,34 @@
       <c r="D11" s="1">
         <v>2.0</v>
       </c>
-      <c r="E11" s="3" t="b">
+      <c r="E11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="3" t="b">
+      <c r="G11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <v>3.0</v>
       </c>
-      <c r="I11" s="3" t="b">
+      <c r="I11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="4">
         <v>2.0</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -924,26 +923,26 @@
       <c r="D12" s="1">
         <v>0.0</v>
       </c>
-      <c r="E12" s="3" t="b">
+      <c r="E12" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="3" t="b">
+      <c r="G12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
         <v>1.0</v>
       </c>
-      <c r="I12" s="3" t="b">
+      <c r="I12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="4">
         <v>1.0</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -951,37 +950,37 @@
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="1">
         <v>0.0</v>
       </c>
-      <c r="E13" s="3" t="b">
+      <c r="E13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="3" t="b">
+      <c r="G13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>1.0</v>
       </c>
-      <c r="I13" s="3" t="b">
+      <c r="I13" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="4">
         <v>1.0</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -989,37 +988,37 @@
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="1">
         <v>1.0</v>
       </c>
-      <c r="E14" s="3" t="b">
+      <c r="E14" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="3" t="b">
+      <c r="G14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
         <v>1.0</v>
       </c>
-      <c r="I14" s="3" t="b">
+      <c r="I14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="4">
         <v>2.0</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1027,37 +1026,37 @@
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="1">
         <v>0.0</v>
       </c>
-      <c r="E15" s="3" t="b">
+      <c r="E15" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="3" t="b">
+      <c r="G15" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="4">
         <v>1.0</v>
       </c>
-      <c r="I15" s="3" t="b">
+      <c r="I15" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="4">
         <v>1.0</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1065,7 +1064,7 @@
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1074,26 +1073,26 @@
       <c r="D16" s="1">
         <v>1.0</v>
       </c>
-      <c r="E16" s="3" t="b">
+      <c r="E16" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="3" t="b">
+      <c r="G16" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="4">
         <v>1.0</v>
       </c>
-      <c r="I16" s="3" t="b">
+      <c r="I16" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="4">
         <v>2.0</v>
       </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1101,7 +1100,7 @@
       <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1110,26 +1109,26 @@
       <c r="D17" s="1">
         <v>0.0</v>
       </c>
-      <c r="E17" s="3" t="b">
+      <c r="E17" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="3" t="b">
+      <c r="G17" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>1.0</v>
       </c>
-      <c r="I17" s="3" t="b">
+      <c r="I17" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="4">
         <v>1.0</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1137,7 +1136,7 @@
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1146,26 +1145,26 @@
       <c r="D18" s="1">
         <v>0.0</v>
       </c>
-      <c r="E18" s="3" t="b">
+      <c r="E18" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="3" t="b">
+      <c r="G18" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
         <v>1.0</v>
       </c>
-      <c r="I18" s="3" t="b">
+      <c r="I18" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="4">
         <v>0.0</v>
       </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3" t="s">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1173,7 +1172,7 @@
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1182,28 +1181,28 @@
       <c r="D19" s="1">
         <v>0.0</v>
       </c>
-      <c r="E19" s="3" t="b">
+      <c r="E19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="3" t="b">
+      <c r="G19" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
         <v>2.0</v>
       </c>
-      <c r="I19" s="3" t="b">
+      <c r="I19" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="4">
         <v>-1.0</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="K19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1211,7 +1210,7 @@
       <c r="A20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1220,28 +1219,28 @@
       <c r="D20" s="1">
         <v>0.0</v>
       </c>
-      <c r="E20" s="3" t="b">
+      <c r="E20" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="3" t="b">
+      <c r="G20" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
         <v>1.0</v>
       </c>
-      <c r="I20" s="3" t="b">
+      <c r="I20" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="4">
         <v>1.0</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1249,35 +1248,35 @@
       <c r="A21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="1">
         <v>1.0</v>
       </c>
-      <c r="E21" s="3" t="b">
+      <c r="E21" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="3" t="b">
+      <c r="G21" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>1.0</v>
       </c>
-      <c r="I21" s="3" t="b">
+      <c r="I21" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="4">
         <v>1.0</v>
       </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3" t="s">
+      <c r="K21" s="4"/>
+      <c r="L21" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1285,37 +1284,37 @@
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="1">
         <v>0.0</v>
       </c>
-      <c r="E22" s="3" t="b">
+      <c r="E22" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="3" t="b">
+      <c r="G22" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="4">
         <v>1.0</v>
       </c>
-      <c r="I22" s="3" t="b">
+      <c r="I22" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="4">
         <v>1.0</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="L22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1323,35 +1322,35 @@
       <c r="A23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="1">
         <v>0.0</v>
       </c>
-      <c r="E23" s="3" t="b">
+      <c r="E23" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="3" t="b">
+      <c r="G23" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
         <v>1.0</v>
       </c>
-      <c r="I23" s="3" t="b">
+      <c r="I23" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="4">
         <v>2.0</v>
       </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3" t="s">
+      <c r="K23" s="4"/>
+      <c r="L23" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1359,35 +1358,35 @@
       <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="1">
         <v>0.0</v>
       </c>
-      <c r="E24" s="3" t="b">
+      <c r="E24" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="3" t="b">
+      <c r="G24" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="4">
         <v>1.0</v>
       </c>
-      <c r="I24" s="3" t="b">
+      <c r="I24" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="4">
         <v>1.0</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3" t="s">
+      <c r="K24" s="4"/>
+      <c r="L24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1395,7 +1394,7 @@
       <c r="A25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1404,26 +1403,26 @@
       <c r="D25" s="1">
         <v>0.0</v>
       </c>
-      <c r="E25" s="3" t="b">
+      <c r="E25" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G25" s="3" t="b">
+      <c r="G25" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="4">
         <v>1.0</v>
       </c>
-      <c r="I25" s="3" t="b">
+      <c r="I25" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="4">
         <v>3.0</v>
       </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3" t="s">
+      <c r="K25" s="4"/>
+      <c r="L25" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1431,7 +1430,7 @@
       <c r="A26" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1440,26 +1439,26 @@
       <c r="D26" s="1">
         <v>0.0</v>
       </c>
-      <c r="E26" s="3" t="b">
+      <c r="E26" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="3" t="b">
+      <c r="G26" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="4">
         <v>1.0</v>
       </c>
-      <c r="I26" s="3" t="b">
+      <c r="I26" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="4">
         <v>2.0</v>
       </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3" t="s">
+      <c r="K26" s="4"/>
+      <c r="L26" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1467,35 +1466,35 @@
       <c r="A27" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="1">
         <v>0.0</v>
       </c>
-      <c r="E27" s="3" t="b">
+      <c r="E27" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="3" t="b">
+      <c r="G27" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="4">
         <v>1.0</v>
       </c>
-      <c r="I27" s="3" t="b">
+      <c r="I27" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="4">
         <v>1.0</v>
       </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3" t="s">
+      <c r="K27" s="4"/>
+      <c r="L27" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1503,35 +1502,35 @@
       <c r="A28" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="1">
         <v>0.0</v>
       </c>
-      <c r="E28" s="3" t="b">
+      <c r="E28" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G28" s="3" t="b">
+      <c r="G28" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="4">
         <v>1.0</v>
       </c>
-      <c r="I28" s="3" t="b">
+      <c r="I28" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="4">
         <v>1.0</v>
       </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3" t="s">
+      <c r="K28" s="4"/>
+      <c r="L28" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1541,7 +1540,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="L29" s="3"/>
+      <c r="L29" s="4"/>
     </row>
     <row r="30">
       <c r="A30" s="2"/>
@@ -8334,7 +8333,6 @@
       <c r="F999" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tutorial fixes related to logging changes
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
   <si>
     <t>Section Text English</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Trigger Count Required</t>
-  </si>
-  <si>
-    <t>Wipe Triggered Objects</t>
   </si>
   <si>
     <t>Save Progress</t>
@@ -490,7 +487,7 @@
     <col customWidth="1" min="6" max="6" width="34.57"/>
     <col customWidth="1" min="7" max="7" width="8.0"/>
     <col customWidth="1" min="8" max="8" width="12.29"/>
-    <col customWidth="1" min="10" max="10" width="10.71"/>
+    <col customWidth="1" min="9" max="9" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -527,9 +524,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -542,17 +537,16 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D2" s="1">
         <v>3.0</v>
@@ -561,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="4" t="b">
         <v>0</v>
@@ -569,26 +563,23 @@
       <c r="H2" s="4">
         <v>1.0</v>
       </c>
-      <c r="I2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="4">
+      <c r="I2" s="4">
         <v>2.0</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
-        <v>16</v>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>0.0</v>
@@ -597,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="4" t="b">
         <v>0</v>
@@ -605,26 +596,23 @@
       <c r="H3" s="4">
         <v>1.0</v>
       </c>
-      <c r="I3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="I3" s="4">
         <v>1.0</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4" t="s">
-        <v>16</v>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D4" s="1">
         <v>0.0</v>
@@ -633,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4" t="b">
         <v>0</v>
@@ -641,28 +629,25 @@
       <c r="H4" s="4">
         <v>1.0</v>
       </c>
-      <c r="I4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I4" s="4">
         <v>3.0</v>
       </c>
+      <c r="J4" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="1">
         <v>0.0</v>
@@ -671,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="4" t="b">
         <v>0</v>
@@ -679,28 +664,25 @@
       <c r="H5" s="4">
         <v>6.0</v>
       </c>
-      <c r="I5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="I5" s="4">
         <v>2.0</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D6" s="1">
         <v>1.0</v>
@@ -709,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="4" t="b">
         <v>0</v>
@@ -717,26 +699,23 @@
       <c r="H6" s="4">
         <v>1.0</v>
       </c>
-      <c r="I6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="I6" s="4">
         <v>1.0</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4" t="s">
-        <v>31</v>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D7" s="1">
         <v>1.0</v>
@@ -745,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="4" t="b">
         <v>0</v>
@@ -753,28 +732,25 @@
       <c r="H7" s="4">
         <v>1.0</v>
       </c>
-      <c r="I7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="I7" s="4">
         <v>0.0</v>
       </c>
+      <c r="J7" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D8" s="1">
         <v>3.0</v>
@@ -783,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="4" t="b">
         <v>0</v>
@@ -791,26 +767,23 @@
       <c r="H8" s="4">
         <v>1.0</v>
       </c>
-      <c r="I8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="I8" s="4">
         <v>1.0</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4" t="s">
-        <v>16</v>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D9" s="1">
         <v>1.0</v>
@@ -819,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="4" t="b">
         <v>1</v>
@@ -827,26 +800,23 @@
       <c r="H9" s="4">
         <v>3.0</v>
       </c>
-      <c r="I9" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="I9" s="4">
         <v>2.0</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4" t="s">
-        <v>16</v>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1">
         <v>0.0</v>
@@ -855,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="4" t="b">
         <v>0</v>
@@ -863,26 +833,23 @@
       <c r="H10" s="4">
         <v>1.0</v>
       </c>
-      <c r="I10" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="I10" s="4">
         <v>1.0</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4" t="s">
-        <v>16</v>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D11" s="1">
         <v>2.0</v>
@@ -891,7 +858,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4" t="b">
         <v>1</v>
@@ -899,26 +866,23 @@
       <c r="H11" s="4">
         <v>3.0</v>
       </c>
-      <c r="I11" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="I11" s="4">
         <v>2.0</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4" t="s">
-        <v>16</v>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1">
         <v>0.0</v>
@@ -927,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="4" t="b">
         <v>0</v>
@@ -935,26 +899,23 @@
       <c r="H12" s="4">
         <v>1.0</v>
       </c>
-      <c r="I12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="I12" s="4">
         <v>1.0</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4" t="s">
-        <v>16</v>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1">
         <v>0.0</v>
@@ -963,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="4" t="b">
         <v>0</v>
@@ -971,28 +932,25 @@
       <c r="H13" s="4">
         <v>1.0</v>
       </c>
-      <c r="I13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="I13" s="4">
         <v>1.0</v>
       </c>
+      <c r="J13" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1">
         <v>1.0</v>
@@ -1001,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="4" t="b">
         <v>0</v>
@@ -1009,28 +967,25 @@
       <c r="H14" s="4">
         <v>1.0</v>
       </c>
-      <c r="I14" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="4">
+      <c r="I14" s="4">
         <v>2.0</v>
       </c>
+      <c r="J14" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1">
         <v>0.0</v>
@@ -1039,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="4" t="b">
         <v>0</v>
@@ -1047,28 +1002,25 @@
       <c r="H15" s="4">
         <v>1.0</v>
       </c>
-      <c r="I15" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" s="4">
+      <c r="I15" s="4">
         <v>1.0</v>
       </c>
+      <c r="J15" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D16" s="1">
         <v>1.0</v>
@@ -1077,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="4" t="b">
         <v>0</v>
@@ -1085,26 +1037,23 @@
       <c r="H16" s="4">
         <v>1.0</v>
       </c>
-      <c r="I16" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="I16" s="4">
         <v>2.0</v>
       </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4" t="s">
-        <v>16</v>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1">
         <v>0.0</v>
@@ -1113,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" s="4" t="b">
         <v>0</v>
@@ -1121,26 +1070,23 @@
       <c r="H17" s="4">
         <v>1.0</v>
       </c>
-      <c r="I17" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4">
+      <c r="I17" s="4">
         <v>1.0</v>
       </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4" t="s">
-        <v>16</v>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D18" s="1">
         <v>0.0</v>
@@ -1149,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G18" s="4" t="b">
         <v>0</v>
@@ -1157,26 +1103,23 @@
       <c r="H18" s="4">
         <v>1.0</v>
       </c>
-      <c r="I18" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4">
+      <c r="I18" s="4">
         <v>0.0</v>
       </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4" t="s">
-        <v>16</v>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D19" s="1">
         <v>0.0</v>
@@ -1185,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19" s="4" t="b">
         <v>1</v>
@@ -1193,28 +1136,25 @@
       <c r="H19" s="4">
         <v>2.0</v>
       </c>
-      <c r="I19" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" s="4">
+      <c r="I19" s="4">
         <v>-1.0</v>
       </c>
+      <c r="J19" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="K19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1">
         <v>0.0</v>
@@ -1223,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G20" s="4" t="b">
         <v>0</v>
@@ -1231,28 +1171,25 @@
       <c r="H20" s="4">
         <v>1.0</v>
       </c>
-      <c r="I20" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" s="4">
+      <c r="I20" s="4">
         <v>1.0</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L20" s="4" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="1">
         <v>1.0</v>
@@ -1261,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G21" s="4" t="b">
         <v>0</v>
@@ -1269,26 +1206,23 @@
       <c r="H21" s="4">
         <v>1.0</v>
       </c>
-      <c r="I21" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" s="4">
+      <c r="I21" s="4">
         <v>1.0</v>
       </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4" t="s">
-        <v>16</v>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1">
         <v>0.0</v>
@@ -1297,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="4" t="b">
         <v>0</v>
@@ -1305,28 +1239,25 @@
       <c r="H22" s="4">
         <v>1.0</v>
       </c>
-      <c r="I22" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" s="4">
+      <c r="I22" s="4">
         <v>1.0</v>
       </c>
+      <c r="J22" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="K22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1">
         <v>0.0</v>
@@ -1335,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" s="4" t="b">
         <v>0</v>
@@ -1343,26 +1274,23 @@
       <c r="H23" s="4">
         <v>1.0</v>
       </c>
-      <c r="I23" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" s="4">
+      <c r="I23" s="4">
         <v>2.0</v>
       </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4" t="s">
-        <v>16</v>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1">
         <v>0.0</v>
@@ -1371,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" s="4" t="b">
         <v>0</v>
@@ -1379,26 +1307,23 @@
       <c r="H24" s="4">
         <v>1.0</v>
       </c>
-      <c r="I24" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" s="4">
+      <c r="I24" s="4">
         <v>1.0</v>
       </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4" t="s">
-        <v>16</v>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="D25" s="1">
         <v>0.0</v>
@@ -1407,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G25" s="4" t="b">
         <v>0</v>
@@ -1415,26 +1340,23 @@
       <c r="H25" s="4">
         <v>1.0</v>
       </c>
-      <c r="I25" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" s="4">
+      <c r="I25" s="4">
         <v>3.0</v>
       </c>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4" t="s">
-        <v>16</v>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D26" s="1">
         <v>0.0</v>
@@ -1443,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G26" s="4" t="b">
         <v>0</v>
@@ -1451,26 +1373,23 @@
       <c r="H26" s="4">
         <v>1.0</v>
       </c>
-      <c r="I26" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="4">
+      <c r="I26" s="4">
         <v>2.0</v>
       </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4" t="s">
-        <v>16</v>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="1">
         <v>0.0</v>
@@ -1479,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>0</v>
@@ -1487,26 +1406,23 @@
       <c r="H27" s="4">
         <v>1.0</v>
       </c>
-      <c r="I27" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J27" s="4">
+      <c r="I27" s="4">
         <v>1.0</v>
       </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4" t="s">
-        <v>16</v>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="C28" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="1">
         <v>0.0</v>
@@ -1515,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G28" s="4" t="b">
         <v>0</v>
@@ -1523,15 +1439,12 @@
       <c r="H28" s="4">
         <v>1.0</v>
       </c>
-      <c r="I28" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" s="4">
+      <c r="I28" s="4">
         <v>1.0</v>
       </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4" t="s">
-        <v>16</v>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29">
@@ -1540,7 +1453,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="L29" s="4"/>
+      <c r="K29" s="4"/>
     </row>
     <row r="30">
       <c r="A30" s="2"/>

</xml_diff>

<commit_message>
Pop-ups handled in TeamSelection split into new their scripts
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Resources/Tutorial/Sports Team Manager Tutorial.xlsx
@@ -164,7 +164,7 @@
     <t>Team Management/Boat Container Bounds/Viewport/Content/Boat</t>
   </si>
   <si>
-    <t>CrewMemberUI, Reset</t>
+    <t>CrewMemberUI, OnReset</t>
   </si>
   <si>
     <t>Once you've filled all of the positions wth crew members, the boat will be ready to take part in the first practice session.</t>
@@ -264,7 +264,7 @@
     <t xml:space="preserve">Questa finestra con i risultati apparirà al termine di ciascuna gara. La gara è andata come ti aspettavi? </t>
   </si>
   <si>
-    <t>TeamSelectionUI, ClosePostRacePopUp</t>
+    <t>RaceResultUI, Close</t>
   </si>
   <si>
     <t>Now you’ve completed your first race and seen where you went right and wrong, it’s time to change things up a little.
@@ -442,49 +442,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>